<commit_message>
Documents\Testing\Test Documents\Test Case Whitebox-group1.xlsx Documents\Testing\Test Documents\Group 1-traceability-matrix.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Testing/Test Documents/Group 1-traceability-matrix.xlsx
+++ b/Documents/Testing/Test Documents/Group 1-traceability-matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A539A7-FAFE-41AA-81C8-0C657EF7C9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBEB8A-9099-45D6-9FD0-D0D54B94D5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="59">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -63,9 +63,6 @@
     <t>R006</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -211,6 +208,12 @@
   </si>
   <si>
     <t>The system must count the number of packages currently in the truck.</t>
+  </si>
+  <si>
+    <t>Whitebox</t>
+  </si>
+  <si>
+    <t>Blackbox</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -331,11 +334,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -349,30 +363,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:U8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,23 +719,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -742,91 +759,91 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
+      <c r="A3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
+      <c r="A4" s="14"/>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
-        <v>14</v>
+      <c r="A5" s="14"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
-        <v>15</v>
+      <c r="A6" s="14"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
-        <v>16</v>
+      <c r="A7" s="14"/>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
-        <v>17</v>
+      <c r="A8" s="14"/>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -834,15 +851,15 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
-        <v>18</v>
+      <c r="A9" s="14"/>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -850,15 +867,15 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
-        <v>19</v>
+      <c r="A10" s="14"/>
+      <c r="B10" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -866,15 +883,15 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11" t="s">
-        <v>20</v>
+      <c r="A11" s="14"/>
+      <c r="B11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -882,15 +899,15 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
+      <c r="A12" s="14"/>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -898,15 +915,15 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11" t="s">
-        <v>22</v>
+      <c r="A13" s="14"/>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -914,15 +931,15 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11" t="s">
-        <v>23</v>
+      <c r="A14" s="14"/>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -930,15 +947,15 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11" t="s">
-        <v>24</v>
+      <c r="A15" s="14"/>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -946,15 +963,15 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11" t="s">
-        <v>25</v>
+      <c r="A16" s="14"/>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -962,15 +979,15 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
-        <v>26</v>
+      <c r="A17" s="14"/>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -978,20 +995,20 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11" t="s">
-        <v>27</v>
+      <c r="A18" s="14"/>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1000,14 +1017,14 @@
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11" t="s">
-        <v>28</v>
+      <c r="A19" s="14"/>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1016,14 +1033,14 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11" t="s">
-        <v>29</v>
+      <c r="A20" s="14"/>
+      <c r="B20" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1032,14 +1049,14 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11" t="s">
-        <v>30</v>
+      <c r="A21" s="14"/>
+      <c r="B21" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1048,14 +1065,14 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="11" t="s">
-        <v>31</v>
+      <c r="A22" s="15"/>
+      <c r="B22" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1064,92 +1081,92 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="10"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="9" t="s">
-        <v>9</v>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="10"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="C24" s="10"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="9" t="s">
-        <v>9</v>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="16"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="9" t="s">
-        <v>9</v>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="16"/>
+      <c r="I25" s="10"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="C26" s="10"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="9" t="s">
-        <v>9</v>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="16"/>
+      <c r="I26" s="10"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="16"/>
+        <v>35</v>
+      </c>
+      <c r="C27" s="10"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="9" t="s">
-        <v>9</v>
+      <c r="E27" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="16"/>
+      <c r="I27" s="10"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1158,12 +1175,12 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1172,12 +1189,12 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1186,12 +1203,12 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1200,12 +1217,12 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1213,151 +1230,761 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="C33" s="10"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
       <c r="B34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="16"/>
+        <v>42</v>
+      </c>
+      <c r="C34" s="10"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
       <c r="B35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="C35" s="10"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
       <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="C36" s="10"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
       <c r="B37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="C37" s="10"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
       <c r="B38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="16"/>
+        <v>46</v>
+      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
       <c r="B39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="16"/>
+        <v>47</v>
+      </c>
+      <c r="C39" s="10"/>
       <c r="D39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
       <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="C40" s="10"/>
       <c r="D40" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
       <c r="B42" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="10"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="2"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="10"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="2"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C71" s="10"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="2"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="9"/>
+      <c r="B72" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H72" s="20"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A47:A66"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C45:J45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1368,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAD6A01-E4C9-46CD-9243-42DE17F0FBE0}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,10 +2007,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1391,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,7 +2026,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1407,7 +2034,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1415,7 +2042,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1423,15 +2050,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,15 +2084,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F850CD00F3C974CA4E11B3B90413122" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8deeb1ecf13acd4d0e51267cabd13c94">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="088f1926-be9f-4f26-b259-435bd2b313b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d40e3588ad538a356041a0b077be6a98" ns3:_="">
     <xsd:import namespace="088f1926-be9f-4f26-b259-435bd2b313b6"/>
@@ -1615,6 +2233,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9EA22A9-AE72-42C9-872A-99948A1A91AC}">
   <ds:schemaRefs>
@@ -1626,14 +2253,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{459B0115-3B1D-44E1-827D-FF38A28C9636}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D66FCE3-CD69-4BAB-B353-DE122C2E8247}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1649,4 +2268,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{459B0115-3B1D-44E1-827D-FF38A28C9636}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Documents\Testing\Test Documents\Final test document-Group1.xlsx Documents\Testing\Test Documents\Group 1-traceability-matrix.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Testing/Test Documents/Group 1-traceability-matrix.xlsx
+++ b/Documents/Testing/Test Documents/Group 1-traceability-matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE1D39E-8B3E-44C7-8D9D-0E0A3D129EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC5AAD4-1740-41EB-8C72-661E8C5004D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="61">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -280,7 +280,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -341,13 +341,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -358,15 +358,32 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -388,9 +405,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,9 +423,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U104" sqref="U104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1860,7 @@
       <c r="I71" s="10"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="13" t="s">
         <v>36</v>
@@ -2197,46 +2215,189 @@
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
     <row r="110" spans="1:10" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="21"/>
+      <c r="B110" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="21"/>
+      <c r="B111" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="21"/>
-    </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="21"/>
-    </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="21"/>
-    </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="21"/>
-    </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="21"/>
-    </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21"/>
-    </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="21"/>
-    </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="21"/>
-    </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="21"/>
-    </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="21"/>
+      <c r="B121" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="9"/>
+      <c r="B122" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H122" s="2"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="9"/>
+      <c r="B123" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="9"/>
+      <c r="B124" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="9"/>
+      <c r="B125" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="9"/>
+      <c r="B126" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="9"/>
+      <c r="B127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H127" s="2"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2263,7 +2424,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="B7" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>